<commit_message>
Created register form, added some example styles, fixed some errors.
</commit_message>
<xml_diff>
--- a/time-capsule-frontend/User-Stories.xlsx
+++ b/time-capsule-frontend/User-Stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nartk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Time Capsule\time-capsule-frontend\time-capsule-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5E5A5F-660E-4027-B5FE-BDE49863A006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CB8E85-23DF-4D02-A1A7-71F935E76CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{82F42668-79FC-4747-B157-EBF04339DDA6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>As a...</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Manage user roles and permissions</t>
+  </si>
+  <si>
+    <t>Sort My Capsules</t>
   </si>
 </sst>
 </file>
@@ -584,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7C9A73-B34B-42BC-A7C5-8A47BEC502B0}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -725,14 +728,14 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
+      <c r="A10" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>5</v>
@@ -743,7 +746,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
@@ -757,12 +760,26 @@
         <v>14</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>